<commit_message>
Corrected Name of Dr. B.T.R. Naresh Reddy
</commit_message>
<xml_diff>
--- a/2nd Year CSE,IT, CSM Timetables.xlsx
+++ b/2nd Year CSE,IT, CSM Timetables.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="100">
   <si>
     <t xml:space="preserve">Aurora's Technological &amp; Research Institute</t>
   </si>
@@ -179,7 +179,7 @@
     <t xml:space="preserve">C++ Lab</t>
   </si>
   <si>
-    <t xml:space="preserve">Dr. Naresh</t>
+    <t xml:space="preserve">Dr. B. T. R. Naresh Reddy</t>
   </si>
   <si>
     <t xml:space="preserve">Mr. Vinod Chavan</t>
@@ -312,9 +312,6 @@
   </si>
   <si>
     <t xml:space="preserve">Dr. O. Vinod Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. B.T.R. Naresh Reddy</t>
   </si>
   <si>
     <t xml:space="preserve">PP Lab</t>
@@ -357,7 +354,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -440,6 +437,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -637,6 +639,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -659,10 +665,6 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -757,7 +759,7 @@
   <dimension ref="A1:K183"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1280,12 +1282,12 @@
       <c r="D28" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
@@ -1510,8 +1512,8 @@
   </sheetPr>
   <dimension ref="A1:K191"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1918,12 +1920,12 @@
       <c r="D22" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
@@ -2032,12 +2034,12 @@
       <c r="D28" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
@@ -2271,7 +2273,7 @@
   </sheetPr>
   <dimension ref="A1:K203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2437,14 +2439,14 @@
       <c r="F10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
       <c r="K10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2487,7 +2489,7 @@
       <c r="D12" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="25" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="15"/>
@@ -2543,7 +2545,7 @@
         <v>18</v>
       </c>
       <c r="F14" s="15"/>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="26" t="s">
         <v>33</v>
       </c>
       <c r="H14" s="14" t="s">
@@ -2812,12 +2814,12 @@
       <c r="D29" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -3253,11 +3255,11 @@
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>
       <c r="G12" s="14" t="s">
@@ -3581,12 +3583,12 @@
       <c r="D29" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -3804,8 +3806,8 @@
   </sheetPr>
   <dimension ref="A1:K197"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3955,11 +3957,11 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="14" t="s">
         <v>28</v>
       </c>
@@ -3984,11 +3986,11 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="14" t="s">
         <v>78</v>
       </c>
@@ -4014,7 +4016,7 @@
       <c r="B12" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="26" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="14" t="s">
@@ -4085,7 +4087,7 @@
       <c r="G14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="26" t="s">
         <v>33</v>
       </c>
       <c r="I14" s="14" t="s">
@@ -4234,7 +4236,7 @@
       <c r="C23" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="19" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="29" t="s">
@@ -4314,7 +4316,7 @@
         <v>81</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
@@ -4330,10 +4332,10 @@
         <v>9</v>
       </c>
       <c r="D28" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="20" t="s">
         <v>90</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>91</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
@@ -4555,7 +4557,7 @@
   </sheetPr>
   <dimension ref="A1:K196"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -4624,7 +4626,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -4652,7 +4654,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -4707,7 +4709,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="30" t="s">
         <v>29</v>
@@ -4733,11 +4735,11 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="14" t="s">
         <v>20</v>
       </c>
@@ -4762,7 +4764,7 @@
         <v>21</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>20</v>
@@ -4772,7 +4774,7 @@
       <c r="G12" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="24" t="s">
         <v>27</v>
       </c>
       <c r="I12" s="14" t="s">
@@ -4785,11 +4787,11 @@
       <c r="A13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="14" t="s">
         <v>28</v>
       </c>
@@ -4813,14 +4815,14 @@
         <v>21</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="15"/>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="23"/>
+      <c r="H14" s="24"/>
       <c r="I14" s="14" t="s">
         <v>28</v>
       </c>
@@ -4837,10 +4839,10 @@
         <v>18</v>
       </c>
       <c r="C15" s="14"/>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="23"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="15"/>
       <c r="G15" s="14" t="s">
         <v>37</v>
@@ -4918,7 +4920,7 @@
         <v>26</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
@@ -4937,7 +4939,7 @@
         <v>42</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
@@ -4955,12 +4957,12 @@
       <c r="D22" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
+      <c r="E22" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
@@ -4972,7 +4974,7 @@
         <v>4</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>45</v>
@@ -5013,7 +5015,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
@@ -5028,11 +5030,11 @@
       <c r="C26" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="19" t="s">
         <v>48</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F26" s="29"/>
       <c r="G26" s="29"/>
@@ -5069,12 +5071,12 @@
       <c r="D28" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
+      <c r="E28" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
@@ -5088,12 +5090,12 @@
       <c r="D29" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
+      <c r="E29" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>

</xml_diff>

<commit_message>
Resolved DS Lab for CSE-2D,IT. Assigned CPE Lab for ECE-1. Assigned PPS-1A to Ms. Keerthi and Kept PPS-1E on Thu(4th Period) from Wednesday. Switched PPS-1D(Mr. Krishna Rao) from Wed(8th Period) to Tue(3rd Period). Replaced Library hour to Seminar hours in the forenoon hours.
</commit_message>
<xml_diff>
--- a/2nd Year CSE,IT, CSM Timetables.xlsx
+++ b/2nd Year CSE,IT, CSM Timetables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CSE-II (A)" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="101">
   <si>
     <t xml:space="preserve">Aurora's Technological &amp; Research Institute</t>
   </si>
@@ -143,6 +143,9 @@
     <t xml:space="preserve">C++ (B1) &amp; ITWS (B2) LAB</t>
   </si>
   <si>
+    <t xml:space="preserve">SEMINAR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thursday</t>
   </si>
   <si>
@@ -354,7 +357,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -438,13 +441,8 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,32 +457,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFA6"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFDBB6"/>
-        <bgColor rgb="FFFFFFA6"/>
       </patternFill>
     </fill>
   </fills>
@@ -550,7 +530,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -603,16 +583,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -635,44 +615,12 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -704,7 +652,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -725,14 +673,14 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFFA6"/>
+      <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFDBB6"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -758,8 +706,8 @@
   </sheetPr>
   <dimension ref="A1:K183"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -912,24 +860,24 @@
       <c r="B10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14" t="s">
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -938,20 +886,20 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="14" t="s">
+      <c r="F11" s="14"/>
+      <c r="G11" s="13" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="13" t="s">
@@ -965,102 +913,102 @@
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="13"/>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="14"/>
+      <c r="I13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="13"/>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="14" t="s">
+      <c r="E14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="14"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="13" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="13"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1106,13 +1054,13 @@
       <c r="A19" s="10"/>
       <c r="B19" s="16"/>
       <c r="C19" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
@@ -1131,7 +1079,7 @@
         <v>26</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
@@ -1147,10 +1095,10 @@
         <v>2</v>
       </c>
       <c r="D21" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>42</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>41</v>
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
@@ -1166,10 +1114,10 @@
         <v>3</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
@@ -1188,7 +1136,7 @@
         <v>19</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
@@ -1207,7 +1155,7 @@
         <v>20</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
@@ -1225,12 +1173,12 @@
       <c r="D25" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="E25" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
@@ -1242,14 +1190,14 @@
         <v>7</v>
       </c>
       <c r="D26" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
@@ -1264,7 +1212,7 @@
         <v>21</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
@@ -1282,12 +1230,12 @@
       <c r="D28" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
+      <c r="E28" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
@@ -1299,10 +1247,10 @@
         <v>10</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
@@ -1512,8 +1460,8 @@
   </sheetPr>
   <dimension ref="A1:K191"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1581,7 +1529,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1609,7 +1557,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -1663,27 +1611,27 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -1692,25 +1640,25 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="14" t="s">
+      <c r="E11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14" t="s">
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="10"/>
@@ -1719,100 +1667,100 @@
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="13"/>
+      <c r="E12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14" t="s">
+      <c r="F12" s="14"/>
+      <c r="G12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14" t="s">
-        <v>24</v>
+      <c r="I12" s="13"/>
+      <c r="J12" s="15" t="s">
+        <v>28</v>
       </c>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="13" t="s">
         <v>29</v>
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13" t="s">
         <v>34</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14" t="s">
-        <v>33</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1858,13 +1806,13 @@
       <c r="A19" s="10"/>
       <c r="B19" s="16"/>
       <c r="C19" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
@@ -1883,7 +1831,7 @@
         <v>26</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
@@ -1899,10 +1847,10 @@
         <v>2</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
@@ -1918,14 +1866,14 @@
         <v>3</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
+      <c r="E22" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
@@ -1940,7 +1888,7 @@
         <v>19</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
@@ -1959,7 +1907,7 @@
         <v>20</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
@@ -1978,7 +1926,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
@@ -1994,14 +1942,14 @@
         <v>7</v>
       </c>
       <c r="D26" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
@@ -2016,7 +1964,7 @@
         <v>21</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
@@ -2034,12 +1982,12 @@
       <c r="D28" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
+      <c r="E28" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
@@ -2051,10 +1999,10 @@
         <v>10</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
@@ -2273,8 +2221,8 @@
   </sheetPr>
   <dimension ref="A1:K203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2342,7 +2290,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2370,7 +2318,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -2424,54 +2372,54 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
+      <c r="H10" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
       <c r="K10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="14" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14" t="s">
+      <c r="I11" s="13"/>
+      <c r="J11" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="10"/>
@@ -2480,100 +2428,100 @@
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14" t="s">
+      <c r="E12" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14" t="s">
+      <c r="I13" s="13"/>
+      <c r="J13" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="H14" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2619,13 +2567,13 @@
       <c r="A19" s="10"/>
       <c r="B19" s="16"/>
       <c r="C19" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
@@ -2644,7 +2592,7 @@
         <v>26</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
@@ -2660,10 +2608,10 @@
         <v>2</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
@@ -2679,10 +2627,10 @@
         <v>3</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
@@ -2701,7 +2649,7 @@
         <v>19</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
@@ -2720,7 +2668,7 @@
         <v>20</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
@@ -2739,7 +2687,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
@@ -2755,10 +2703,10 @@
         <v>7</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
@@ -2777,7 +2725,7 @@
         <v>21</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
@@ -2796,7 +2744,7 @@
         <v>27</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
@@ -2812,14 +2760,14 @@
         <v>10</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
+        <v>51</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -3046,8 +2994,8 @@
   </sheetPr>
   <dimension ref="A1:K194"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3115,7 +3063,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3143,7 +3091,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -3197,27 +3145,27 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -3226,123 +3174,127 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="14" t="s">
+      <c r="F11" s="14"/>
+      <c r="G11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="14"/>
+      <c r="I11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="13"/>
       <c r="K11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14" t="s">
+      <c r="B12" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14" t="s">
+      <c r="H13" s="13"/>
+      <c r="I13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="14" t="s">
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3388,13 +3340,13 @@
       <c r="A19" s="10"/>
       <c r="B19" s="16"/>
       <c r="C19" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
@@ -3413,7 +3365,7 @@
         <v>26</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
@@ -3429,10 +3381,10 @@
         <v>2</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
@@ -3448,10 +3400,10 @@
         <v>3</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
@@ -3470,7 +3422,7 @@
         <v>19</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
@@ -3489,7 +3441,7 @@
         <v>20</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
@@ -3508,7 +3460,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
@@ -3524,10 +3476,10 @@
         <v>7</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
@@ -3546,7 +3498,7 @@
         <v>21</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
@@ -3565,7 +3517,7 @@
         <v>27</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
@@ -3581,14 +3533,14 @@
         <v>10</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
+        <v>51</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -3806,8 +3758,8 @@
   </sheetPr>
   <dimension ref="A1:K197"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3875,7 +3827,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3903,7 +3855,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -3957,27 +3909,27 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="15" t="s">
+      <c r="B10" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="I10" s="14" t="s">
+      <c r="H10" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="I10" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -3986,26 +3938,26 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="14" t="s">
+      <c r="F11" s="14"/>
+      <c r="G11" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="14" t="s">
-        <v>24</v>
+      <c r="J11" s="15" t="s">
+        <v>28</v>
       </c>
       <c r="K11" s="10"/>
     </row>
@@ -4013,106 +3965,106 @@
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="14" t="s">
+      <c r="B12" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14" t="s">
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="J12" s="14" t="s">
+      <c r="H12" s="13"/>
+      <c r="I12" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J12" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" s="14" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="I13" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="J13" s="14" t="s">
+      <c r="H13" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="J14" s="14"/>
+      <c r="I14" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J14" s="13"/>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="B15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4158,13 +4110,13 @@
       <c r="A19" s="10"/>
       <c r="B19" s="16"/>
       <c r="C19" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
@@ -4180,10 +4132,10 @@
         <v>1</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
@@ -4202,7 +4154,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
@@ -4221,7 +4173,7 @@
         <v>18</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
@@ -4237,14 +4189,14 @@
         <v>4</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
+        <v>49</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
@@ -4256,10 +4208,10 @@
         <v>5</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
@@ -4275,10 +4227,10 @@
         <v>6</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
@@ -4294,10 +4246,10 @@
         <v>7</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
@@ -4313,10 +4265,10 @@
         <v>8</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
@@ -4332,10 +4284,10 @@
         <v>9</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
@@ -4557,8 +4509,8 @@
   </sheetPr>
   <dimension ref="A1:K196"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4626,7 +4578,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -4654,7 +4606,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -4708,25 +4660,25 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" s="30" t="s">
+      <c r="B10" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="15" t="s">
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="31" t="s">
+      <c r="H10" s="13"/>
+      <c r="I10" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -4735,23 +4687,23 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="14" t="s">
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="14" t="s">
+      <c r="F11" s="14"/>
+      <c r="G11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14" t="s">
+      <c r="H11" s="13"/>
+      <c r="I11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="10"/>
@@ -4760,96 +4712,96 @@
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="14" t="s">
+      <c r="C12" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14" t="s">
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="14"/>
+      <c r="I12" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="13"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="24" t="s">
+      <c r="D14" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="24"/>
-      <c r="I14" s="14" t="s">
+      <c r="H14" s="13"/>
+      <c r="I14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="24" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4895,13 +4847,13 @@
       <c r="A19" s="10"/>
       <c r="B19" s="16"/>
       <c r="C19" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
@@ -4920,7 +4872,7 @@
         <v>26</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
@@ -4936,10 +4888,10 @@
         <v>2</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
@@ -4955,14 +4907,14 @@
         <v>3</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
+        <v>44</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
@@ -4974,10 +4926,10 @@
         <v>4</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
@@ -4996,7 +4948,7 @@
         <v>20</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
@@ -5015,7 +4967,7 @@
         <v>18</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
@@ -5031,14 +4983,14 @@
         <v>7</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
+        <v>49</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
@@ -5053,7 +5005,7 @@
         <v>21</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
@@ -5071,12 +5023,12 @@
       <c r="D28" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
+      <c r="E28" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
@@ -5088,14 +5040,14 @@
         <v>10</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
+        <v>51</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>

</xml_diff>

<commit_message>
DS(2-IT) updated for Ms. Lakshmi
</commit_message>
<xml_diff>
--- a/2nd Year CSE,IT, CSM Timetables.xlsx
+++ b/2nd Year CSE,IT, CSM Timetables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="CSE-II (A)" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="101">
   <si>
     <t xml:space="preserve">Aurora's Technological &amp; Research Institute</t>
   </si>
@@ -457,14 +457,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF81D41A"/>
-        <bgColor rgb="FF969696"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -530,7 +530,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -591,7 +591,7 @@
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -615,12 +615,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -706,8 +710,8 @@
   </sheetPr>
   <dimension ref="A1:K183"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -947,7 +951,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="13"/>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="15" t="s">
         <v>27</v>
       </c>
       <c r="F13" s="14"/>
@@ -1674,7 +1678,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="13"/>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F12" s="14"/>
@@ -2222,7 +2226,7 @@
   <dimension ref="A1:K203"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2995,7 +2999,7 @@
   <dimension ref="A1:K194"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3758,8 +3762,8 @@
   </sheetPr>
   <dimension ref="A1:K197"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4510,7 +4514,7 @@
   <dimension ref="A1:K196"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4660,24 +4664,24 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="23" t="s">
-        <v>26</v>
-      </c>
+      <c r="I10" s="23"/>
       <c r="J10" s="13" t="s">
         <v>24</v>
       </c>
@@ -4699,7 +4703,9 @@
       <c r="G11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="23" t="s">
+        <v>94</v>
+      </c>
       <c r="I11" s="13" t="s">
         <v>18</v>
       </c>
@@ -4766,10 +4772,12 @@
       <c r="C14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="13"/>
       <c r="F14" s="14"/>
       <c r="G14" s="13" t="s">
         <v>27</v>
@@ -5222,21 +5230,19 @@
     <row r="195" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="196" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="27">
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="F10:F15"/>
-    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:H11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="G13:I13"/>
-    <mergeCell ref="D14:E14"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:E15"/>

</xml_diff>

<commit_message>
Tentative time table before preparing 3-2 time table
</commit_message>
<xml_diff>
--- a/2nd Year CSE,IT, CSM Timetables.xlsx
+++ b/2nd Year CSE,IT, CSM Timetables.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="104">
   <si>
     <t xml:space="preserve">Aurora's Technological &amp; Research Institute</t>
   </si>
@@ -101,34 +101,115 @@
     <t xml:space="preserve">Monday</t>
   </si>
   <si>
+    <t xml:space="preserve">OOPC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L U N C H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADE (B1) &amp; C++ (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPORTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEMINAR</t>
+  </si>
+  <si>
     <t xml:space="preserve">DS</t>
   </si>
   <si>
-    <t xml:space="preserve">COA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COSM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L U N C H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADE (B1) &amp; C++ (B2) LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPORTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tuesday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OOPC</t>
+    <t xml:space="preserve">ITWS (B1) &amp; ADE (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C++ (B1) &amp; DS (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thursday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MENTORING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS (B1) &amp; ITWS (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saturday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTRA CURRICULAR ACTIVITIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faculty Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Sirisha Tumma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADE Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C++ Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. B. T. R. Naresh Reddy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. Vinod Chavan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Gita S Parthiban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. Rohit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. V Swetha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. Ch. Krishna Rao (B1) &amp; Ms. S Anitha (B2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSE-II (B)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room No: A216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITWS (B1) &amp; DS (B2) LAB</t>
   </si>
   <si>
     <t xml:space="preserve">LIB</t>
@@ -137,88 +218,16 @@
     <t xml:space="preserve">DS (B1) &amp; ADE (B2) LAB</t>
   </si>
   <si>
-    <t xml:space="preserve">Wednesday</t>
-  </si>
-  <si>
     <t xml:space="preserve">C++ (B1) &amp; ITWS (B2) LAB</t>
   </si>
   <si>
-    <t xml:space="preserve">SEMINAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thursday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MENTORING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Friday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITWS (B1) &amp; DS (B2) LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saturday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXTRA CURRICULAR ACTIVITIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S.No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faculty Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. Sirisha Tumma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADE Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C++ Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. B. T. R. Naresh Reddy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr. Vinod Chavan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. Gita S Parthiban</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr. Rohit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. V Swetha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITWS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. TV Ramanamma (B1) &amp; Ms. S Anitha (B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE-II (B)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Room No: A216</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ms. K Aparna</t>
   </si>
   <si>
     <t xml:space="preserve">Dr. O Vinod Kumar</t>
   </si>
   <si>
-    <t xml:space="preserve">Ms. Sameena (B1) &amp; Ms. A. Anitha (B2)</t>
+    <t xml:space="preserve">Ms. Vineela (B1) &amp; Ms. Gowthami (B2)</t>
   </si>
   <si>
     <t xml:space="preserve">CSE-II (C)</t>
@@ -233,9 +242,6 @@
     <t xml:space="preserve">ITWS (B1) &amp; C++ (B2) LAB</t>
   </si>
   <si>
-    <t xml:space="preserve">C++ (B1) &amp; DS (B2) LAB</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mr. Sunkari Rajasheker</t>
   </si>
   <si>
@@ -335,7 +341,13 @@
     <t xml:space="preserve">Ms. Nuzhath Farhana</t>
   </si>
   <si>
+    <t xml:space="preserve">Ms. D. Bhavani</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ms. Vineela (B1) &amp; (B2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. K. Thrisandhya</t>
   </si>
   <si>
     <t xml:space="preserve">Ms. P. Lakshmi</t>
@@ -454,6 +466,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
@@ -462,12 +480,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF81D41A"/>
         <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -533,7 +545,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -586,6 +598,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -614,7 +630,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -622,16 +642,12 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -714,7 +730,7 @@
   <dimension ref="A1:K183"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -867,24 +883,24 @@
       <c r="B10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13" t="s">
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -893,19 +909,19 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="13" t="s">
         <v>28</v>
       </c>
@@ -925,97 +941,97 @@
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="13" t="s">
+      <c r="E12" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="F12" s="15"/>
+      <c r="G12" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="13"/>
+      <c r="J13" s="14"/>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>35</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>36</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="13" t="s">
+      <c r="E14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1059,209 +1075,209 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="E19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18" t="n">
+      <c r="B20" s="18"/>
+      <c r="C20" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+      <c r="E20" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18" t="n">
+      <c r="B21" s="18"/>
+      <c r="C21" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="19" t="s">
+      <c r="D21" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
+      <c r="E21" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18" t="n">
+      <c r="B22" s="18"/>
+      <c r="C22" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18" t="n">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="E23" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18" t="n">
+      <c r="B24" s="18"/>
+      <c r="C24" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
+      <c r="E24" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18" t="n">
+      <c r="B25" s="18"/>
+      <c r="C25" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
+      <c r="D25" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18" t="n">
+      <c r="B26" s="18"/>
+      <c r="C26" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="19" t="s">
+      <c r="D26" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
+      <c r="E26" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18" t="n">
+      <c r="B27" s="18"/>
+      <c r="C27" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
+      <c r="E27" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18" t="n">
+      <c r="B28" s="18"/>
+      <c r="C28" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="D28" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18" t="n">
+      <c r="B29" s="18"/>
+      <c r="C29" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E29" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -1468,7 +1484,7 @@
   <dimension ref="A1:K191"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="K28" activeCellId="0" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1536,7 +1552,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1564,7 +1580,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -1618,27 +1634,27 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13" t="s">
+      <c r="G10" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -1648,24 +1664,22 @@
         <v>25</v>
       </c>
       <c r="B11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="13" t="s">
+      <c r="F11" s="15"/>
+      <c r="G11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13" t="s">
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="10"/>
@@ -1674,100 +1688,102 @@
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13" t="s">
+      <c r="C12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="13" t="s">
+      <c r="F12" s="15"/>
+      <c r="G12" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13" t="s">
-        <v>28</v>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13" t="s">
+      <c r="F13" s="15"/>
+      <c r="G13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="F14" s="15"/>
+      <c r="G14" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13" t="s">
-        <v>34</v>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="13" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1811,209 +1827,209 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="E19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18" t="n">
+      <c r="B20" s="18"/>
+      <c r="C20" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+      <c r="E20" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18" t="n">
+      <c r="B21" s="18"/>
+      <c r="C21" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
+      <c r="D21" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18" t="n">
+      <c r="B22" s="18"/>
+      <c r="C22" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18" t="n">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="E23" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18" t="n">
+      <c r="B24" s="18"/>
+      <c r="C24" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
+      <c r="E24" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18" t="n">
+      <c r="B25" s="18"/>
+      <c r="C25" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
+      <c r="D25" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18" t="n">
+      <c r="B26" s="18"/>
+      <c r="C26" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="19" t="s">
+      <c r="D26" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
+      <c r="E26" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18" t="n">
+      <c r="B27" s="18"/>
+      <c r="C27" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
+      <c r="E27" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18" t="n">
+      <c r="B28" s="18"/>
+      <c r="C28" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="D28" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18" t="n">
+      <c r="B29" s="18"/>
+      <c r="C29" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
+      <c r="D29" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -2190,15 +2206,15 @@
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="F10:F15"/>
     <mergeCell ref="G10:I10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C12:D12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="E19:H19"/>
     <mergeCell ref="E20:H20"/>
     <mergeCell ref="E21:H21"/>
@@ -2297,7 +2313,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2325,7 +2341,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -2379,54 +2395,54 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="14" t="s">
+      <c r="E10" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
+      <c r="G10" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
       <c r="K10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13" t="s">
+      <c r="I11" s="14"/>
+      <c r="J11" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="10"/>
@@ -2435,100 +2451,100 @@
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="13" t="s">
+      <c r="F12" s="15"/>
+      <c r="G12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
+      <c r="H12" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="13" t="s">
+      <c r="B13" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="F13" s="15"/>
+      <c r="G13" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13" t="s">
+      <c r="I13" s="14"/>
+      <c r="J13" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
+      <c r="E14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2572,209 +2588,209 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="E19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18" t="n">
+      <c r="B20" s="18"/>
+      <c r="C20" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+      <c r="E20" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18" t="n">
+      <c r="B21" s="18"/>
+      <c r="C21" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
+      <c r="D21" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18" t="n">
+      <c r="B22" s="18"/>
+      <c r="C22" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="D22" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18" t="n">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="E23" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18" t="n">
+      <c r="B24" s="18"/>
+      <c r="C24" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
+      <c r="E24" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18" t="n">
+      <c r="B25" s="18"/>
+      <c r="C25" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
+      <c r="D25" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18" t="n">
+      <c r="B26" s="18"/>
+      <c r="C26" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
+      <c r="D26" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18" t="n">
+      <c r="B27" s="18"/>
+      <c r="C27" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
+      <c r="E27" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18" t="n">
+      <c r="B28" s="18"/>
+      <c r="C28" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="D28" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18" t="n">
+      <c r="B29" s="18"/>
+      <c r="C29" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
+      <c r="D29" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -3002,7 +3018,7 @@
   <dimension ref="A1:K194"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3070,7 +3086,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3098,7 +3114,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -3152,27 +3168,27 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13" t="s">
+      <c r="B10" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="13" t="s">
+      <c r="H10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -3181,127 +3197,127 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="C11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="13" t="s">
+      <c r="F11" s="15"/>
+      <c r="G11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="13"/>
+      <c r="I11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="14"/>
       <c r="K11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="13" t="s">
+      <c r="B12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13" t="s">
+      <c r="B13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="13" t="s">
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3345,209 +3361,209 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="E19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18" t="n">
+      <c r="B20" s="18"/>
+      <c r="C20" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+      <c r="E20" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18" t="n">
+      <c r="B21" s="18"/>
+      <c r="C21" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
+      <c r="D21" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18" t="n">
+      <c r="B22" s="18"/>
+      <c r="C22" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="D22" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18" t="n">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="E23" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18" t="n">
+      <c r="B24" s="18"/>
+      <c r="C24" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
+      <c r="E24" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18" t="n">
+      <c r="B25" s="18"/>
+      <c r="C25" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
+      <c r="D25" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18" t="n">
+      <c r="B26" s="18"/>
+      <c r="C26" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
+      <c r="D26" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18" t="n">
+      <c r="B27" s="18"/>
+      <c r="C27" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
+      <c r="E27" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18" t="n">
+      <c r="B28" s="18"/>
+      <c r="C28" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="D28" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18" t="n">
+      <c r="B29" s="18"/>
+      <c r="C29" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
+      <c r="D29" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -3834,7 +3850,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3862,7 +3878,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -3916,27 +3932,27 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="14" t="s">
+      <c r="B10" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="J10" s="13" t="s">
+      <c r="H10" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -3945,26 +3961,26 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="13" t="s">
+      <c r="I11" s="14" t="s">
         <v>28</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="K11" s="10"/>
     </row>
@@ -3972,106 +3988,106 @@
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="13" t="s">
+      <c r="B12" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="J12" s="13" t="s">
+      <c r="H12" s="14"/>
+      <c r="I12" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="13" t="s">
+      <c r="C13" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="13" t="s">
+      <c r="E13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="H13" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="J14" s="13"/>
+      <c r="H14" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="14"/>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4115,190 +4131,190 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="E19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18" t="n">
+      <c r="B20" s="18"/>
+      <c r="C20" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="19" t="s">
+      <c r="D20" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+      <c r="E20" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18" t="n">
+      <c r="B21" s="18"/>
+      <c r="C21" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
+      <c r="E21" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18" t="n">
+      <c r="B22" s="18"/>
+      <c r="C22" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="D22" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18" t="n">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="D23" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18" t="n">
+      <c r="B24" s="18"/>
+      <c r="C24" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
+      <c r="D24" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18" t="n">
+      <c r="B25" s="18"/>
+      <c r="C25" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
+      <c r="D25" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18" t="n">
+      <c r="B26" s="18"/>
+      <c r="C26" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
+      <c r="D26" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18" t="n">
+      <c r="B27" s="18"/>
+      <c r="C27" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
+      <c r="D27" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18" t="n">
+      <c r="B28" s="18"/>
+      <c r="C28" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="D28" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
@@ -4517,7 +4533,7 @@
   <dimension ref="A1:K196"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4585,7 +4601,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -4613,7 +4629,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -4667,25 +4683,25 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="14" t="s">
+      <c r="C10" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="13" t="s">
+      <c r="G10" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="24"/>
+      <c r="J10" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -4694,25 +4710,25 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13" t="s">
+      <c r="B11" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="13" t="s">
+      <c r="F11" s="15"/>
+      <c r="G11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="13" t="s">
+      <c r="H11" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="10"/>
@@ -4721,98 +4737,98 @@
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="D12" s="13" t="s">
+      <c r="C12" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="13" t="s">
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="13"/>
+      <c r="H12" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="14"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="13" t="s">
+      <c r="B13" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="J14" s="13" t="s">
+      <c r="E14" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="14" t="s">
         <v>24</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4856,209 +4872,209 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="E19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18" t="n">
+      <c r="B20" s="18"/>
+      <c r="C20" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
+      <c r="E20" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18" t="n">
+      <c r="B21" s="18"/>
+      <c r="C21" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
+      <c r="D21" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18" t="n">
+      <c r="B22" s="18"/>
+      <c r="C22" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
+      <c r="D22" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18" t="n">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="D23" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18" t="n">
+      <c r="B24" s="18"/>
+      <c r="C24" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
+      <c r="E24" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18" t="n">
+      <c r="B25" s="18"/>
+      <c r="C25" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
+      <c r="D25" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18" t="n">
+      <c r="B26" s="18"/>
+      <c r="C26" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
+      <c r="D26" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18" t="n">
+      <c r="B27" s="18"/>
+      <c r="C27" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
+      <c r="E27" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18" t="n">
+      <c r="B28" s="18"/>
+      <c r="C28" s="19" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
+      <c r="D28" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18" t="n">
+      <c r="B29" s="18"/>
+      <c r="C29" s="19" t="n">
         <v>10</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
+      <c r="D29" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>

</xml_diff>

<commit_message>
Tentative time table for 3rd years
</commit_message>
<xml_diff>
--- a/2nd Year CSE,IT, CSM Timetables.xlsx
+++ b/2nd Year CSE,IT, CSM Timetables.xlsx
@@ -104,27 +104,30 @@
     <t xml:space="preserve">OOPC</t>
   </si>
   <si>
+    <t xml:space="preserve">COSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L U N C H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADE (B1) &amp; C++ (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPORTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuesday</t>
+  </si>
+  <si>
     <t xml:space="preserve">COA</t>
   </si>
   <si>
-    <t xml:space="preserve">COSM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L U N C H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADE (B1) &amp; C++ (B2) LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPORTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tuesday</t>
-  </si>
-  <si>
     <t xml:space="preserve">ADE</t>
   </si>
   <si>
@@ -333,9 +336,6 @@
   </si>
   <si>
     <t xml:space="preserve">Room No: A214C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COM</t>
   </si>
   <si>
     <t xml:space="preserve">Ms. Nuzhath Farhana</t>
@@ -451,7 +451,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -474,12 +474,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF81D41A"/>
-        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -545,7 +539,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -598,6 +592,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -630,8 +628,12 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -640,10 +642,6 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -703,7 +701,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF81D41A"/>
+      <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -730,7 +728,7 @@
   <dimension ref="A1:K183"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -889,18 +887,18 @@
       <c r="D10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14" t="s">
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -909,24 +907,24 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="C11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="D11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="15"/>
+      <c r="E11" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="16"/>
       <c r="G11" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
@@ -934,104 +932,104 @@
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="14"/>
+      <c r="I13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="15"/>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="14" t="s">
+      <c r="H14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1075,209 +1073,209 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="17" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="D19" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="E19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19" t="n">
+      <c r="B20" s="19"/>
+      <c r="C20" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
+      <c r="D20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19" t="n">
+      <c r="B21" s="19"/>
+      <c r="C21" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19" t="n">
+      <c r="B22" s="19"/>
+      <c r="C22" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="20" t="s">
+      <c r="D22" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
+      <c r="E22" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19" t="n">
+      <c r="B23" s="19"/>
+      <c r="C23" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="D23" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19" t="n">
+      <c r="B24" s="19"/>
+      <c r="C24" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
+      <c r="D24" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19" t="n">
+      <c r="B25" s="19"/>
+      <c r="C25" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
+      <c r="D25" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19" t="n">
+      <c r="B26" s="19"/>
+      <c r="C26" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19" t="n">
+      <c r="B27" s="19"/>
+      <c r="C27" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
+      <c r="E27" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19" t="n">
+      <c r="B28" s="19"/>
+      <c r="C28" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
+      <c r="E28" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19" t="n">
+      <c r="B29" s="19"/>
+      <c r="C29" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="21" t="s">
+      <c r="D29" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
+      <c r="E29" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -1484,7 +1482,7 @@
   <dimension ref="A1:K191"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K28" activeCellId="0" sqref="K28"/>
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1552,7 +1550,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1580,7 +1578,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -1634,27 +1632,27 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>26</v>
+      <c r="B10" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="15" t="s">
+      <c r="E10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14" t="s">
+      <c r="G10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -1664,126 +1662,126 @@
         <v>25</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="13"/>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="14" t="s">
+      <c r="F11" s="23"/>
+      <c r="G11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14" t="s">
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="G12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14" t="s">
+      <c r="H12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14" t="s">
-        <v>55</v>
+      <c r="I12" s="13"/>
+      <c r="J12" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14" t="s">
+      <c r="E13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="15" t="s">
         <v>34</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14" t="s">
-        <v>33</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H15" s="13"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1827,209 +1825,209 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="17" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="D19" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="E19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19" t="n">
+      <c r="B20" s="19"/>
+      <c r="C20" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
+      <c r="D20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19" t="n">
+      <c r="B21" s="19"/>
+      <c r="C21" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="D21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19" t="n">
+      <c r="B22" s="19"/>
+      <c r="C22" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="20" t="s">
+      <c r="D22" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
+      <c r="E22" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19" t="n">
+      <c r="B23" s="19"/>
+      <c r="C23" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="D23" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19" t="n">
+      <c r="B24" s="19"/>
+      <c r="C24" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
+      <c r="D24" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19" t="n">
+      <c r="B25" s="19"/>
+      <c r="C25" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
+      <c r="D25" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19" t="n">
+      <c r="B26" s="19"/>
+      <c r="C26" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19" t="n">
+      <c r="B27" s="19"/>
+      <c r="C27" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
+      <c r="E27" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19" t="n">
+      <c r="B28" s="19"/>
+      <c r="C28" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
+      <c r="E28" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19" t="n">
+      <c r="B29" s="19"/>
+      <c r="C29" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
+      <c r="D29" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -2313,7 +2311,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2341,7 +2339,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -2395,156 +2393,156 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="G10" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14" t="s">
+      <c r="I11" s="15"/>
+      <c r="J11" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="14" t="s">
+      <c r="C12" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="E12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14" t="s">
+      <c r="H13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="H14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2588,209 +2586,209 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="17" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="D19" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="E19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19" t="n">
+      <c r="B20" s="19"/>
+      <c r="C20" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
+      <c r="D20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19" t="n">
+      <c r="B21" s="19"/>
+      <c r="C21" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="D21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19" t="n">
+      <c r="B22" s="19"/>
+      <c r="C22" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
+      <c r="D22" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19" t="n">
+      <c r="B23" s="19"/>
+      <c r="C23" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="D23" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19" t="n">
+      <c r="B24" s="19"/>
+      <c r="C24" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
+      <c r="D24" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19" t="n">
+      <c r="B25" s="19"/>
+      <c r="C25" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
+      <c r="D25" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19" t="n">
+      <c r="B26" s="19"/>
+      <c r="C26" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
+      <c r="D26" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19" t="n">
+      <c r="B27" s="19"/>
+      <c r="C27" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
+      <c r="E27" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19" t="n">
+      <c r="B28" s="19"/>
+      <c r="C28" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
+      <c r="E28" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19" t="n">
+      <c r="B29" s="19"/>
+      <c r="C29" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
+      <c r="D29" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -3086,7 +3084,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3114,7 +3112,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -3168,27 +3166,27 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14" t="s">
+      <c r="B10" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="14" t="s">
+      <c r="I10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -3197,127 +3195,127 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="14"/>
+      <c r="I11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="15"/>
       <c r="K11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="14" t="s">
+      <c r="F13" s="16"/>
+      <c r="G13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="14" t="s">
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="14" t="s">
+      <c r="H14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="I14" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3361,209 +3359,209 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="17" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="D19" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="E19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19" t="n">
+      <c r="B20" s="19"/>
+      <c r="C20" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
+      <c r="D20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19" t="n">
+      <c r="B21" s="19"/>
+      <c r="C21" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="D21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19" t="n">
+      <c r="B22" s="19"/>
+      <c r="C22" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
+      <c r="D22" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19" t="n">
+      <c r="B23" s="19"/>
+      <c r="C23" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="D23" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19" t="n">
+      <c r="B24" s="19"/>
+      <c r="C24" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
+      <c r="D24" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19" t="n">
+      <c r="B25" s="19"/>
+      <c r="C25" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
+      <c r="D25" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19" t="n">
+      <c r="B26" s="19"/>
+      <c r="C26" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
+      <c r="D26" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19" t="n">
+      <c r="B27" s="19"/>
+      <c r="C27" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
+      <c r="E27" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19" t="n">
+      <c r="B28" s="19"/>
+      <c r="C28" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
+      <c r="E28" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19" t="n">
+      <c r="B29" s="19"/>
+      <c r="C29" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
+      <c r="D29" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -3850,7 +3848,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3878,7 +3876,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -3932,27 +3930,27 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="15" t="s">
+      <c r="B10" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="14" t="s">
+      <c r="G10" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="I10" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -3961,133 +3959,133 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14" t="s">
+      <c r="F11" s="16"/>
+      <c r="G11" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>55</v>
+      <c r="I11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="K11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="J12" s="14" t="s">
+      <c r="D12" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="J12" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="H13" s="14" t="s">
+      <c r="E13" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="I13" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="J13" s="14" t="s">
+      <c r="H13" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="J14" s="14"/>
+      <c r="I14" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="J14" s="15"/>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="B15" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4131,190 +4129,190 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="17" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="D19" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="E19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19" t="n">
+      <c r="B20" s="19"/>
+      <c r="C20" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
+      <c r="D20" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19" t="n">
+      <c r="B21" s="19"/>
+      <c r="C21" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="D21" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19" t="n">
+      <c r="B22" s="19"/>
+      <c r="C22" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
+      <c r="D22" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19" t="n">
+      <c r="B23" s="19"/>
+      <c r="C23" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="D23" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19" t="n">
+      <c r="B24" s="19"/>
+      <c r="C24" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
+      <c r="D24" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19" t="n">
+      <c r="B25" s="19"/>
+      <c r="C25" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="E25" s="20" t="s">
+      <c r="D25" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
+      <c r="E25" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19" t="n">
+      <c r="B26" s="19"/>
+      <c r="C26" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
+      <c r="D26" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19" t="n">
+      <c r="B27" s="19"/>
+      <c r="C27" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
+      <c r="D27" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19" t="n">
+      <c r="B28" s="19"/>
+      <c r="C28" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E28" s="20" t="s">
+      <c r="D28" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
+      <c r="E28" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
@@ -4533,7 +4531,7 @@
   <dimension ref="A1:K196"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4601,7 +4599,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -4629,7 +4627,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -4683,25 +4681,25 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="15" t="s">
+      <c r="B10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="14" t="s">
+      <c r="G10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -4710,125 +4708,125 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14" t="s">
+      <c r="B11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="14" t="s">
+      <c r="I11" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="D12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="14" t="s">
+      <c r="D12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="14"/>
+      <c r="I12" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="13"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="15"/>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="14" t="s">
+      <c r="F14" s="23"/>
+      <c r="G14" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="J14" s="14" t="s">
+      <c r="H14" s="13"/>
+      <c r="I14" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="15" t="s">
         <v>24</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4872,209 +4870,209 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="17" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="D19" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="E19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19" t="n">
+      <c r="B20" s="19"/>
+      <c r="C20" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="20" t="s">
+      <c r="D20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19" t="n">
+      <c r="B21" s="19"/>
+      <c r="C21" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="20" t="s">
+      <c r="D21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19" t="n">
+      <c r="B22" s="19"/>
+      <c r="C22" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="20" t="s">
+      <c r="D22" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19" t="n">
+      <c r="B23" s="19"/>
+      <c r="C23" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="20" t="s">
+      <c r="D23" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19" t="n">
+      <c r="B24" s="19"/>
+      <c r="C24" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
+      <c r="D24" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19" t="n">
+      <c r="B25" s="19"/>
+      <c r="C25" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="20" t="s">
+      <c r="D25" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19" t="n">
+      <c r="B26" s="19"/>
+      <c r="C26" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="20" t="s">
+      <c r="D26" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19" t="n">
+      <c r="B27" s="19"/>
+      <c r="C27" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
+      <c r="E27" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19" t="n">
+      <c r="B28" s="19"/>
+      <c r="C28" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19" t="n">
+      <c r="B29" s="19"/>
+      <c r="C29" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
+      <c r="D29" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>

</xml_diff>

<commit_message>
Workload of Ms. Srija is given to Ms. Mamatha.
</commit_message>
<xml_diff>
--- a/2nd Year CSE,IT, CSM Timetables.xlsx
+++ b/2nd Year CSE,IT, CSM Timetables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CSE-II (A)" sheetId="1" state="visible" r:id="rId2"/>
@@ -107,235 +107,235 @@
     <t xml:space="preserve">COSM</t>
   </si>
   <si>
+    <t xml:space="preserve">COA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L U N C H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADE (B1) &amp; C++ (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPORTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEMINAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITWS (B1) &amp; ADE (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wednesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C++ (B1) &amp; DS (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thursday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MENTORING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS (B1) &amp; ITWS (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saturday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTRA CURRICULAR ACTIVITIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faculty Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Sirisha Tumma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADE Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C++ Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. B. T. R. Naresh Reddy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. Vinod Chavan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Gita S Parthiban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. Rohit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. V Swetha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Mamatha (B1) &amp; Ms.S Anitha (B2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSE-II (B)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room No: A216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITWS (B1) &amp; DS (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS (B1) &amp; ADE (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C++ (B1) &amp; ITWS (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. K Aparna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. O Vinod Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Vineela (B1) &amp; Ms. Gowthami (B2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSE-II (C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room No: A204A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADE (B1) &amp; ITWS (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITWS (B1) &amp; C++ (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. Sunkari Rajasheker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. K Rajini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. D Venugopal Reddy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. P Lakshmi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr.Akash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Gowthami (B1) &amp; (B2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSE-II (D)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room No: A101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. K Thrisandya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. Md. Nizamuddin Salman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. P Laxmi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. Mamatha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSM-II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room No: A204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS (B1) &amp; PP (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PP(B1) &amp; DS (B2) LAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEFA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. E. Navya Sree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. K. Rajini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. Masood Ahmed (B1) &amp; (B2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. D. Saritha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GS Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. V. Swetha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. O. Vinod Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PP Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ms. G. Keerthi (B1) &amp; Ms. Subhashini (B2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT-II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room No: A214C</t>
+  </si>
+  <si>
     <t xml:space="preserve">COM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L U N C H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADE (B1) &amp; C++ (B2) LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPORTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tuesday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEMINAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITWS (B1) &amp; ADE (B2) LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wednesday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C++ (B1) &amp; DS (B2) LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thursday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MENTORING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Friday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS (B1) &amp; ITWS (B2) LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saturday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXTRA CURRICULAR ACTIVITIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S.No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faculty Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. Sirisha Tumma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADE Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C++ Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. B. T. R. Naresh Reddy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr. Vinod Chavan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. Gita S Parthiban</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr. Rohit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. V Swetha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITWS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr. Ch. Krishna Rao (B1) &amp; Ms. S Anitha (B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE-II (B)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Room No: A216</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITWS (B1) &amp; DS (B2) LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS (B1) &amp; ADE (B2) LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C++ (B1) &amp; ITWS (B2) LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. K Aparna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. O Vinod Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. Vineela (B1) &amp; Ms. Gowthami (B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE-II (C)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Room No: A204A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADE (B1) &amp; ITWS (B2) LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITWS (B1) &amp; C++ (B2) LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr. Sunkari Rajasheker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. K Rajini</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr. D Venugopal Reddy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. P Lakshmi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr.Akash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. Gowthami (B1) &amp; (B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE-II (D)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Room No: A101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. K Thrisandya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. Md. Nizamuddin Salman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. P Laxmi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. Srija (B1) &amp; (B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSM-II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Room No: A204</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DS (B1) &amp; PP (B2) LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PP(B1) &amp; DS (B2) LAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BEFA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. E. Navya Sree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. K. Rajini</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. Masood Ahmed (B1) &amp; (B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. D. Saritha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GS Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. V. Swetha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dr. O. Vinod Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PP Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ms. G. Keerthi (B1) &amp; Ms. Subhashini (B2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT-II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Room No: A214C</t>
   </si>
   <si>
     <t xml:space="preserve">Ms. Nuzhath Farhana</t>
@@ -539,7 +539,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -596,14 +596,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -628,12 +620,12 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -728,7 +720,7 @@
   <dimension ref="A1:K183"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -881,24 +873,24 @@
       <c r="B10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15" t="s">
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -907,24 +899,24 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="E11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="F11" s="14"/>
+      <c r="G11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="13" t="s">
+      <c r="H11" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>30</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
@@ -932,104 +924,104 @@
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>32</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="15" t="s">
+      <c r="E12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12" s="15" t="s">
+      <c r="I12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="15"/>
+      <c r="J13" s="13"/>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>35</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>36</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="15" t="s">
+      <c r="E14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="F14" s="14"/>
+      <c r="G14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="H14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="J14" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1073,209 +1065,209 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="E19" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20" t="n">
+      <c r="B20" s="17"/>
+      <c r="C20" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
+      <c r="D20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20" t="n">
+      <c r="B21" s="17"/>
+      <c r="C21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="21" t="s">
+      <c r="D21" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="E21" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20" t="n">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20" t="n">
+      <c r="B23" s="17"/>
+      <c r="C23" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
+      <c r="D23" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20" t="n">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
+      <c r="E24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20" t="n">
+      <c r="B25" s="17"/>
+      <c r="C25" s="18" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="D25" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20" t="n">
+      <c r="B26" s="17"/>
+      <c r="C26" s="18" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="21" t="s">
+      <c r="D26" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
+      <c r="E26" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20" t="n">
+      <c r="B27" s="17"/>
+      <c r="C27" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
+      <c r="E27" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20" t="n">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
+      <c r="E28" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="20" t="n">
+      <c r="B29" s="17"/>
+      <c r="C29" s="18" t="n">
         <v>10</v>
       </c>
       <c r="D29" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E29" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -1550,7 +1542,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1578,7 +1570,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -1633,10 +1625,10 @@
         <v>17</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>18</v>
@@ -1644,15 +1636,15 @@
       <c r="E10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="14" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -1662,7 +1654,7 @@
         <v>25</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13" t="s">
@@ -1671,86 +1663,86 @@
       <c r="E11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="23"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
-      <c r="J11" s="15" t="s">
+      <c r="J11" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="23"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I12" s="13"/>
-      <c r="J12" s="15" t="s">
-        <v>56</v>
+      <c r="J12" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="E13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="23"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="23"/>
+        <v>27</v>
+      </c>
+      <c r="F14" s="14"/>
       <c r="G14" s="13" t="s">
         <v>18</v>
       </c>
@@ -1758,30 +1750,30 @@
         <v>19</v>
       </c>
       <c r="I14" s="13"/>
-      <c r="J14" s="15" t="s">
-        <v>34</v>
+      <c r="J14" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="13"/>
-      <c r="F15" s="23"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H15" s="13"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1825,209 +1817,209 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="E19" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20" t="n">
+      <c r="B20" s="17"/>
+      <c r="C20" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
+      <c r="D20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20" t="n">
+      <c r="B21" s="17"/>
+      <c r="C21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="D21" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20" t="n">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20" t="n">
+      <c r="B23" s="17"/>
+      <c r="C23" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
+      <c r="D23" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20" t="n">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
+      <c r="E24" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20" t="n">
+      <c r="B25" s="17"/>
+      <c r="C25" s="18" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="D25" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20" t="n">
+      <c r="B26" s="17"/>
+      <c r="C26" s="18" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="21" t="s">
+      <c r="D26" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
+      <c r="E26" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20" t="n">
+      <c r="B27" s="17"/>
+      <c r="C27" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
+      <c r="E27" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20" t="n">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
+      <c r="E28" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="20" t="n">
+      <c r="B29" s="17"/>
+      <c r="C29" s="18" t="n">
         <v>10</v>
       </c>
-      <c r="D29" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
+      <c r="D29" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -2242,7 +2234,7 @@
   </sheetPr>
   <dimension ref="A1:K203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -2311,7 +2303,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2339,7 +2331,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -2393,156 +2385,156 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
+      <c r="G10" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
       <c r="K10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15" t="s">
+      <c r="B11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="15" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15" t="s">
+      <c r="I11" s="13"/>
+      <c r="J11" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="15" t="s">
+      <c r="F12" s="14"/>
+      <c r="G12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
+      <c r="H12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15" t="s">
+      <c r="H13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
+      <c r="D14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2586,209 +2578,209 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="E19" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20" t="n">
+      <c r="B20" s="17"/>
+      <c r="C20" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
+      <c r="D20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20" t="n">
+      <c r="B21" s="17"/>
+      <c r="C21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="D21" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20" t="n">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="D22" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20" t="n">
+      <c r="B23" s="17"/>
+      <c r="C23" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
+      <c r="D23" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20" t="n">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
+      <c r="E24" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20" t="n">
+      <c r="B25" s="17"/>
+      <c r="C25" s="18" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="D25" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20" t="n">
+      <c r="B26" s="17"/>
+      <c r="C26" s="18" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
+      <c r="D26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20" t="n">
+      <c r="B27" s="17"/>
+      <c r="C27" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
+      <c r="E27" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20" t="n">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
+      <c r="E28" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="20" t="n">
+      <c r="B29" s="17"/>
+      <c r="C29" s="18" t="n">
         <v>10</v>
       </c>
-      <c r="D29" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
+      <c r="D29" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>
@@ -3016,7 +3008,7 @@
   <dimension ref="A1:K194"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3084,7 +3076,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3112,7 +3104,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -3166,27 +3158,27 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15" t="s">
+      <c r="B10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -3195,127 +3187,127 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="15" t="s">
+      <c r="F11" s="14"/>
+      <c r="G11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="15"/>
+      <c r="I11" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="13"/>
       <c r="K11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15" t="s">
+      <c r="H13" s="13"/>
+      <c r="I13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="15" t="s">
+      <c r="C14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="15" t="s">
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" s="15" t="s">
+      <c r="J14" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3359,205 +3351,205 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="E19" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20" t="n">
+      <c r="B20" s="17"/>
+      <c r="C20" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
+      <c r="D20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20" t="n">
+      <c r="B21" s="17"/>
+      <c r="C21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="D21" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20" t="n">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="D22" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20" t="n">
+      <c r="B23" s="17"/>
+      <c r="C23" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
+      <c r="D23" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20" t="n">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
+      <c r="E24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20" t="n">
+      <c r="B25" s="17"/>
+      <c r="C25" s="18" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="D25" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20" t="n">
+      <c r="B26" s="17"/>
+      <c r="C26" s="18" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
+      <c r="D26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20" t="n">
+      <c r="B27" s="17"/>
+      <c r="C27" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
+      <c r="E27" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20" t="n">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
+      <c r="E28" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="20" t="n">
+      <c r="B29" s="17"/>
+      <c r="C29" s="18" t="n">
         <v>10</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
@@ -3848,7 +3840,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3876,7 +3868,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -3930,27 +3922,27 @@
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="15" t="s">
+      <c r="I10" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -3959,133 +3951,133 @@
       <c r="A11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>56</v>
+      <c r="H11" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="K11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="J12" s="15" t="s">
+      <c r="J12" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="C14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="15" t="s">
+      <c r="F14" s="14"/>
+      <c r="G14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="J14" s="15"/>
+      <c r="H14" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="13"/>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4129,190 +4121,190 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="E19" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20" t="n">
+      <c r="B20" s="17"/>
+      <c r="C20" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
+      <c r="D20" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20" t="n">
+      <c r="B21" s="17"/>
+      <c r="C21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="D21" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20" t="n">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="D22" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20" t="n">
+      <c r="B23" s="17"/>
+      <c r="C23" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
+      <c r="D23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20" t="n">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
+      <c r="D24" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20" t="n">
+      <c r="B25" s="17"/>
+      <c r="C25" s="18" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20" t="n">
+      <c r="B26" s="17"/>
+      <c r="C26" s="18" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
+      <c r="D26" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20" t="n">
+      <c r="B27" s="17"/>
+      <c r="C27" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
+      <c r="D27" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20" t="n">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="E28" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
@@ -4530,7 +4522,7 @@
   </sheetPr>
   <dimension ref="A1:K196"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -4599,7 +4591,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -4627,7 +4619,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>5</v>
@@ -4682,24 +4674,24 @@
         <v>17</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="14" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" s="13"/>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="10"/>
@@ -4709,79 +4701,79 @@
         <v>25</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="23"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="13"/>
-      <c r="F12" s="23"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>18</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J12" s="13"/>
       <c r="K12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="23"/>
+        <v>27</v>
+      </c>
+      <c r="F13" s="14"/>
       <c r="G13" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
-      <c r="J13" s="15"/>
+      <c r="J13" s="13"/>
       <c r="K13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>19</v>
@@ -4790,43 +4782,43 @@
         <v>21</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="23"/>
+        <v>96</v>
+      </c>
+      <c r="F14" s="14"/>
       <c r="G14" s="13" t="s">
         <v>18</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="J14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4870,209 +4862,209 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="E19" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="10"/>
       <c r="J19" s="0"/>
       <c r="K19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20" t="n">
+      <c r="B20" s="17"/>
+      <c r="C20" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="21" t="s">
+      <c r="D20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
       <c r="I20" s="10"/>
       <c r="J20" s="0"/>
       <c r="K20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20" t="n">
+      <c r="B21" s="17"/>
+      <c r="C21" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="D21" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="21" t="s">
+      <c r="D21" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
       <c r="I21" s="10"/>
       <c r="J21" s="0"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20" t="n">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="21" t="s">
+      <c r="D22" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
       <c r="I22" s="10"/>
       <c r="J22" s="0"/>
       <c r="K22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20" t="n">
+      <c r="B23" s="17"/>
+      <c r="C23" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="21" t="s">
+      <c r="D23" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
       <c r="I23" s="10"/>
       <c r="J23" s="0"/>
       <c r="K23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20" t="n">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
+      <c r="E24" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
       <c r="I24" s="10"/>
       <c r="J24" s="0"/>
       <c r="K24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20" t="n">
+      <c r="B25" s="17"/>
+      <c r="C25" s="18" t="n">
         <v>6</v>
       </c>
-      <c r="D25" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="21" t="s">
+      <c r="D25" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="10"/>
       <c r="J25" s="0"/>
       <c r="K25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20" t="n">
+      <c r="B26" s="17"/>
+      <c r="C26" s="18" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="21" t="s">
+      <c r="D26" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="10"/>
       <c r="J26" s="0"/>
       <c r="K26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20" t="n">
+      <c r="B27" s="17"/>
+      <c r="C27" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
+      <c r="E27" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
       <c r="I27" s="10"/>
       <c r="J27" s="0"/>
       <c r="K27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20" t="n">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18" t="n">
         <v>9</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
       <c r="I28" s="10"/>
       <c r="J28" s="0"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="20" t="n">
+      <c r="B29" s="17"/>
+      <c r="C29" s="18" t="n">
         <v>10</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
+        <v>50</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
       <c r="I29" s="10"/>
       <c r="J29" s="0"/>
       <c r="K29" s="10"/>

</xml_diff>